<commit_message>
changing around the assignments and ProjectAssignments and also adding differnt ways to calc the times - estimated time by hours and recommended time by days
</commit_message>
<xml_diff>
--- a/data/assignments.xlsx
+++ b/data/assignments.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$E$1:$F$54</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="77">
   <si>
     <t xml:space="preserve">step</t>
   </si>
@@ -31,7 +34,7 @@
     <t xml:space="preserve">estimated_time</t>
   </si>
   <si>
-    <t xml:space="preserve">recommended_start_date</t>
+    <t xml:space="preserve">recommended_start_offset</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
@@ -40,18 +43,18 @@
     <t xml:space="preserve">target_audience</t>
   </si>
   <si>
+    <t xml:space="preserve">is_on_going</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_day_of</t>
+  </si>
+  <si>
     <t xml:space="preserve">הגדרה ראשונית</t>
   </si>
   <si>
     <t xml:space="preserve">הגדרת מטרות הכנס</t>
   </si>
   <si>
-    <t xml:space="preserve">1–2 שעות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6–9 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">פרונטלי, וירטואלי, היברידי</t>
   </si>
   <si>
@@ -67,123 +70,63 @@
     <t xml:space="preserve">בניית תקציב ראשוני</t>
   </si>
   <si>
-    <t xml:space="preserve">3–5 שעות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6–8 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">גיוס צוות מארגן</t>
   </si>
   <si>
-    <t xml:space="preserve">2-4 ימים</t>
-  </si>
-  <si>
     <t xml:space="preserve">תכנון תוכן</t>
   </si>
   <si>
     <t xml:space="preserve">ניסוח קול קורא</t>
   </si>
   <si>
-    <t xml:space="preserve">2–4 שעות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5–7 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">פתיחת מערכת להגשת תקצירים</t>
   </si>
   <si>
-    <t xml:space="preserve">2–3 שעות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5–6 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">וירטואלי, היברידי</t>
   </si>
   <si>
     <t xml:space="preserve">חיפוש וגיוס סוקרים</t>
   </si>
   <si>
-    <t xml:space="preserve">4–2 שבועות</t>
-  </si>
-  <si>
     <t xml:space="preserve">תיאום עם keynote speakers</t>
   </si>
   <si>
-    <t xml:space="preserve">1-2 שבועות</t>
-  </si>
-  <si>
     <t xml:space="preserve">בינ"ל</t>
   </si>
   <si>
     <t xml:space="preserve">גיוס מנחים לפאנלים</t>
   </si>
   <si>
-    <t xml:space="preserve">1 שבועות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4–5 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">בניית לו"ז הכנס</t>
   </si>
   <si>
-    <t xml:space="preserve">2-3 ימים</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2–3 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">תכנון סדנאות והרצאות</t>
   </si>
   <si>
     <t xml:space="preserve">איסוף מצגות</t>
   </si>
   <si>
-    <t xml:space="preserve">2–3 שבועות</t>
-  </si>
-  <si>
     <t xml:space="preserve">פרסום לו"ז הכנס</t>
   </si>
   <si>
-    <t xml:space="preserve">1–2 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">יצירת תעודות השתתפות</t>
   </si>
   <si>
-    <t xml:space="preserve">שבוע–שבועיים</t>
-  </si>
-  <si>
     <t xml:space="preserve">לוגיסטיקה</t>
   </si>
   <si>
     <t xml:space="preserve">מציאת מקום</t>
   </si>
   <si>
-    <t xml:space="preserve">2-6 שבועות</t>
-  </si>
-  <si>
     <t xml:space="preserve">פרונטלי, היברידי</t>
   </si>
   <si>
     <t xml:space="preserve">סידורי לינה</t>
   </si>
   <si>
-    <t xml:space="preserve">3–5 שבועות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3–4 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">שירותי חנייה</t>
   </si>
   <si>
-    <t xml:space="preserve">2–3 ימים</t>
-  </si>
-  <si>
     <t xml:space="preserve">הזמנת קייטרינג</t>
   </si>
   <si>
@@ -193,27 +136,21 @@
     <t xml:space="preserve">שירותי אבטחה</t>
   </si>
   <si>
+    <t xml:space="preserve">ביום הכנס</t>
+  </si>
+  <si>
     <t xml:space="preserve">שי למשתתפים</t>
   </si>
   <si>
-    <t xml:space="preserve">2 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">ערכות למשתתף (לרבות דיגיטליות)</t>
   </si>
   <si>
-    <t xml:space="preserve">חודש</t>
-  </si>
-  <si>
     <t xml:space="preserve">הדפסת שילוט</t>
   </si>
   <si>
     <t xml:space="preserve">גיוס דיילים</t>
   </si>
   <si>
-    <t xml:space="preserve">2–1 שבועות</t>
-  </si>
-  <si>
     <t xml:space="preserve">מענה רפואי</t>
   </si>
   <si>
@@ -226,9 +163,6 @@
     <t xml:space="preserve">תיאום תחזוקה (כיסאות, שולחנות, מקרנים)/ שטח</t>
   </si>
   <si>
-    <t xml:space="preserve">שבוע</t>
-  </si>
-  <si>
     <t xml:space="preserve">שיווק ופרסום</t>
   </si>
   <si>
@@ -241,48 +175,24 @@
     <t xml:space="preserve">מתמשך</t>
   </si>
   <si>
-    <t xml:space="preserve">מהרגע שנפתח הרישום</t>
+    <t xml:space="preserve">Y</t>
   </si>
   <si>
     <t xml:space="preserve">יצירת ושליחת הזמנות</t>
   </si>
   <si>
-    <t xml:space="preserve">2–4 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">בניית רשימות תפוצה</t>
   </si>
   <si>
-    <t xml:space="preserve">3–5 חודשים</t>
-  </si>
-  <si>
     <t xml:space="preserve">שליחת ניוזלטרים</t>
   </si>
   <si>
-    <t xml:space="preserve">1–2 פעמים לשליחה</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 חודשים עד שבוע לפני</t>
-  </si>
-  <si>
     <t xml:space="preserve">פרסום ברשתות</t>
   </si>
   <si>
-    <t xml:space="preserve">1–2 פעמים בחודש</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 חודשים ועד יום הכנס</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ביום הכנס</t>
-  </si>
-  <si>
     <t xml:space="preserve">עמדת רישום</t>
   </si>
   <si>
-    <t xml:space="preserve">ביום האירוע</t>
-  </si>
-  <si>
     <t xml:space="preserve">דוכן מידע</t>
   </si>
   <si>
@@ -295,18 +205,12 @@
     <t xml:space="preserve">מענה לבלת"מים</t>
   </si>
   <si>
-    <t xml:space="preserve">לפי צורך</t>
-  </si>
-  <si>
     <t xml:space="preserve">הקלטות / שידור</t>
   </si>
   <si>
     <t xml:space="preserve">תיעוד / צילום</t>
   </si>
   <si>
-    <t xml:space="preserve">1-2 שעות</t>
-  </si>
-  <si>
     <t xml:space="preserve">חלוקת תגי שמות</t>
   </si>
   <si>
@@ -316,52 +220,40 @@
     <t xml:space="preserve">וידוא הגעת ספקים</t>
   </si>
   <si>
-    <t xml:space="preserve">2-3 שעות</t>
-  </si>
-  <si>
     <t xml:space="preserve">לאחר הכנס</t>
   </si>
   <si>
     <t xml:space="preserve">כתיבת ושליחת משוב</t>
   </si>
   <si>
-    <t xml:space="preserve">4–2 שעות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">יום–יומיים לאחר הכנס</t>
-  </si>
-  <si>
     <t xml:space="preserve">ניתוח נתונים</t>
   </si>
   <si>
-    <t xml:space="preserve">2–1 שעות</t>
-  </si>
-  <si>
-    <t xml:space="preserve">עד שבוע</t>
-  </si>
-  <si>
     <t xml:space="preserve">דו"ח מסכם</t>
   </si>
   <si>
-    <t xml:space="preserve">תוך שבועיים</t>
-  </si>
-  <si>
     <t xml:space="preserve">תודות</t>
   </si>
   <si>
-    <t xml:space="preserve">תוך שבוע</t>
-  </si>
-  <si>
     <t xml:space="preserve">פרסום חומרים</t>
   </si>
   <si>
-    <t xml:space="preserve">עד שבועיים</t>
-  </si>
-  <si>
     <t xml:space="preserve">תיעוד תובנות</t>
   </si>
   <si>
-    <t xml:space="preserve">עד חודש</t>
+    <t xml:space="preserve"> תכנון עמדת רישום</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> תכנון דוכן מידע</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ארגון הקלטות / שידור</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ארגון  תגי שמות</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ארגון שי למשתתפים</t>
   </si>
 </sst>
 </file>
@@ -371,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +296,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="177"/>
     </font>
   </fonts>
   <fills count="2">
@@ -455,7 +354,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -468,6 +367,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +380,28 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,23 +581,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="42.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="44.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="32.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,7 +611,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -695,19 +620,25 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>182</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>10</v>
@@ -718,16 +649,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
+      <c r="C3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>182</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -738,16 +669,16 @@
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
+      <c r="C4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>10</v>
@@ -758,16 +689,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>16</v>
+      <c r="C5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>182</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -778,16 +709,16 @@
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>182</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
@@ -798,39 +729,39 @@
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
@@ -838,56 +769,56 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>504</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>120</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
@@ -898,16 +829,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
@@ -918,16 +849,16 @@
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>90</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
@@ -938,16 +869,16 @@
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>90</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
@@ -958,16 +889,16 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>10</v>
@@ -978,16 +909,16 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>10</v>
@@ -998,59 +929,59 @@
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>672</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>182</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>672</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>120</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>11</v>
@@ -1058,19 +989,19 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>11</v>
@@ -1078,19 +1009,19 @@
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -1098,19 +1029,19 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>11</v>
@@ -1118,19 +1049,19 @@
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>11</v>
@@ -1138,16 +1069,16 @@
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>30</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>10</v>
@@ -1158,19 +1089,19 @@
     </row>
     <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>11</v>
@@ -1178,19 +1109,19 @@
     </row>
     <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>11</v>
@@ -1198,19 +1129,19 @@
     </row>
     <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>60</v>
+        <v>42</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>11</v>
@@ -1218,19 +1149,19 @@
     </row>
     <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>60</v>
+        <v>43</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>11</v>
@@ -1238,19 +1169,19 @@
     </row>
     <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>68</v>
+      <c r="C29" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>11</v>
@@ -1258,16 +1189,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>504</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>120</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>10</v>
@@ -1278,36 +1209,39 @@
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>90</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>10</v>
@@ -1318,16 +1252,16 @@
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>77</v>
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>120</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>10</v>
@@ -1338,116 +1272,131 @@
     </row>
     <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>80</v>
+        <v>49</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>120</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>83</v>
+        <v>49</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>86</v>
+        <v>55</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>10</v>
@@ -1455,82 +1404,94 @@
       <c r="F39" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H39" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>86</v>
+        <v>62</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>36</v>
+        <v>64</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>11</v>
@@ -1538,16 +1499,16 @@
     </row>
     <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>102</v>
+        <v>66</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>-2</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>10</v>
@@ -1558,16 +1519,16 @@
     </row>
     <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>105</v>
+        <v>67</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>-7</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>10</v>
@@ -1578,16 +1539,16 @@
     </row>
     <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>107</v>
+        <v>68</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>-14</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>10</v>
@@ -1598,16 +1559,16 @@
     </row>
     <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>109</v>
+        <v>69</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <v>-7</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>10</v>
@@ -1618,16 +1579,16 @@
     </row>
     <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>111</v>
+        <v>70</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>-14</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>10</v>
@@ -1638,16 +1599,16 @@
     </row>
     <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>113</v>
+        <v>71</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>-30</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>10</v>
@@ -1656,7 +1617,137 @@
         <v>11</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>336</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="E1:F54">
+    <filterColumn colId="0">
+      <customFilters and="true">
+        <customFilter operator="equal" val="*פרונטלי*"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="לוקלי, בינ&quot;ל"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1664,5 +1755,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>